<commit_message>
updated per task 431389
</commit_message>
<xml_diff>
--- a/organize/raci-template.xlsx
+++ b/organize/raci-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brblanch\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoftapc-my.sharepoint.com/personal/ronelv_microsoft_com/Documents/Microsoft Teams Chat Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B8FA09A-F092-47F1-84B4-33B8A2EA4A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="8_{ACACD675-5BAE-40FB-B2B0-0DD77C38D9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A80E210E-62F5-48A5-8769-7863CA1A18FC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{AB571973-26AF-4BE6-A95F-82C0E308CB25}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{AB571973-26AF-4BE6-A95F-82C0E308CB25}"/>
   </bookViews>
   <sheets>
     <sheet name="Org Alignment" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="122">
   <si>
     <t>Define high level alignment of required capabilities across the org structure</t>
   </si>
@@ -556,30 +565,6 @@
   </si>
   <si>
     <t>Microsoft Azure Well-Architected Framework,Azure Advisor Score, Landing Zone Templates</t>
-  </si>
-  <si>
-    <t>Cloud Security</t>
-  </si>
-  <si>
-    <t>Manage and operate the security posture</t>
-  </si>
-  <si>
-    <t>Leadership</t>
-  </si>
-  <si>
-    <t>Posture &amp; Compliance</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Cloud security team</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>CCoE-Cloud security</t>
   </si>
 </sst>
 </file>
@@ -685,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -907,6 +892,21 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1178,7 +1178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1209,14 +1209,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
@@ -1270,13 +1271,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1285,91 +1286,91 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1484,13 +1485,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>375808</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>147768</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1829,53 +1830,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB8EBB1-C082-49F7-95F1-16A7569FC7E5}">
-  <dimension ref="B1:J35"/>
+  <dimension ref="B1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.54296875" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" customWidth="1"/>
-    <col min="5" max="5" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="40.53125" customWidth="1"/>
+    <col min="4" max="4" width="27.265625" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" customWidth="1"/>
-    <col min="8" max="8" width="16.7265625" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="20.265625" customWidth="1"/>
+    <col min="8" max="8" width="16.73046875" customWidth="1"/>
+    <col min="9" max="9" width="19.19921875" customWidth="1"/>
+    <col min="10" max="10" width="17.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="90" t="s">
+    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="92"/>
-    </row>
-    <row r="3" spans="2:10" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="37"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+    </row>
+    <row r="3" spans="2:10" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B3" s="38"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
@@ -1895,8 +1896,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="32" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B5" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1907,8 +1908,8 @@
       <c r="F5" s="2"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B6" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1919,8 +1920,8 @@
       <c r="F6" s="2"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1931,8 +1932,8 @@
       <c r="F7" s="2"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B8" s="33" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1943,8 +1944,8 @@
       <c r="F8" s="2"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="32" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B9" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1955,131 +1956,133 @@
       <c r="F9" s="2"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="32" t="s">
-        <v>122</v>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B10" s="33" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="33" t="s">
+    <row r="11" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="90" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="2:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="93" t="s">
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="95"/>
-    </row>
-    <row r="16" spans="2:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="88" t="s">
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
+      <c r="J14" s="96"/>
+    </row>
+    <row r="15" spans="2:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="85" t="s">
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="87"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="37"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="38"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="88"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B16" s="38"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="88"/>
+    </row>
+    <row r="17" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B17" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>4</v>
+      </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="87"/>
-    </row>
-    <row r="18" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="36"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="19" t="s">
+      <c r="G17" s="35"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B18" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C18" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G18" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H18" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J18" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B19" s="11"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12"/>
+      <c r="G19" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="25"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" s="11"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -2088,26 +2091,26 @@
         <v>13</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="25"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" s="11"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="12"/>
       <c r="G21" s="24" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="25"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" s="11"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -2116,26 +2119,26 @@
         <v>19</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="25"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="11"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="12"/>
       <c r="G23" s="24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="25"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="11"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -2144,12 +2147,12 @@
         <v>21</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="25"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="11"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2158,12 +2161,12 @@
         <v>21</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="25"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="11"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -2172,26 +2175,26 @@
         <v>21</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="25"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="11"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="12"/>
       <c r="G27" s="24" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="25"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="11"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -2200,26 +2203,26 @@
         <v>15</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="25"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B29" s="11"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="12"/>
       <c r="G29" s="24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="25"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -2228,78 +2231,52 @@
         <v>11</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="25"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B31" s="11"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="12"/>
-      <c r="G31" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>48</v>
-      </c>
+      <c r="G31" s="24"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="25"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B32" s="11"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="12"/>
-      <c r="G32" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="G32" s="24"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="25"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B33" s="11"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="12"/>
-      <c r="G33" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="25"/>
-    </row>
-    <row r="34" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="15"/>
-      <c r="G34" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
-    </row>
-    <row r="35" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
+    </row>
+    <row r="34" spans="2:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="G16:J17"/>
-    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="G15:J16"/>
+    <mergeCell ref="B15:E15"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="G14:J14"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D12" xr:uid="{413798D1-14CC-49B8-BDBB-05FC1C736071}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D11" xr:uid="{413798D1-14CC-49B8-BDBB-05FC1C736071}">
       <formula1>"""Align to org structure"", ""Planned alignment"",  ""Not needed"", ""To be evaluated"", "</formula1>
     </dataValidation>
   </dataValidations>
@@ -2309,12 +2286,11 @@
     <hyperlink ref="B7" r:id="rId3" xr:uid="{F83D6C1A-A1AD-4037-B3B1-06923B4D0276}"/>
     <hyperlink ref="B8" r:id="rId4" xr:uid="{EE1058B6-9BD3-40FB-8288-1C65BB7F2B24}"/>
     <hyperlink ref="B9" r:id="rId5" xr:uid="{1B3B4551-1D96-4690-A3FA-72E549C64BFE}"/>
-    <hyperlink ref="B11" r:id="rId6" xr:uid="{125496A0-20BD-4FEB-AF09-F7381CB360F5}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{367B5135-8B18-4C27-A7E0-8B259C5CAD6E}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{D15CE963-4F62-4302-A01F-59F42D5A85CE}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{125496A0-20BD-4FEB-AF09-F7381CB360F5}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{367B5135-8B18-4C27-A7E0-8B259C5CAD6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2326,155 +2302,155 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.19921875" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" customWidth="1"/>
+    <col min="5" max="5" width="20.53125" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" customWidth="1"/>
+    <col min="7" max="7" width="14.53125" customWidth="1"/>
+    <col min="8" max="8" width="15.53125" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:10" ht="28.5" x14ac:dyDescent="0.85">
+      <c r="B2" s="29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="33.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29" t="s">
+    <row r="4" spans="2:10" ht="33.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="30" t="s">
+    <row r="5" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="30" t="s">
+      <c r="G5" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="30" t="s">
+    <row r="6" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-    </row>
-    <row r="8" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B8" s="30" t="s">
+    <row r="7" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+    </row>
+    <row r="8" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B8" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>71</v>
       </c>
@@ -2482,7 +2458,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>73</v>
       </c>
@@ -2490,7 +2466,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>75</v>
       </c>
@@ -2498,7 +2474,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>77</v>
       </c>
@@ -2526,381 +2502,323 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72EF455-C7C4-4BE0-B05C-CCAD85B1AB1E}">
-  <dimension ref="B2:K25"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.19921875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" customWidth="1"/>
-    <col min="7" max="8" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" customWidth="1"/>
+    <col min="5" max="5" width="20.53125" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" customWidth="1"/>
+    <col min="7" max="7" width="14.53125" customWidth="1"/>
+    <col min="8" max="8" width="15.53125" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:10" ht="28.5" x14ac:dyDescent="0.85">
+      <c r="B2" s="29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="33.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29" t="s">
+    <row r="5" spans="2:10" ht="33.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="I5" s="29" t="s">
+      <c r="H5" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="I5" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="J5" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="30" t="s">
+    <row r="6" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="30" t="s">
+      <c r="F6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="I6" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="J6" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="30" t="s">
+    <row r="7" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="30" t="s">
+      <c r="D7" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="30" t="s">
+      <c r="F7" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="30" t="s">
+    </row>
+    <row r="8" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="30" t="s">
+      <c r="I8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="J9" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="30" t="s">
+      <c r="I10" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="E11" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-    </row>
-    <row r="14" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="30" t="s">
+    </row>
+    <row r="12" spans="2:10" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C13" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D13" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E13" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F13" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G13" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="I14" s="31" t="s">
+      <c r="H13" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="I13" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="J13" s="32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{3234C89B-9AB2-478E-9316-4F988EA27559}"/>
-    <hyperlink ref="C14" r:id="rId2" xr:uid="{3945B433-F36A-47F7-81F3-3217A70B44EA}"/>
-    <hyperlink ref="D14" r:id="rId3" xr:uid="{66EC8D73-7E0C-46A6-B289-AC037C945EBA}"/>
-    <hyperlink ref="E14" r:id="rId4" xr:uid="{37E5CC3F-B59C-4D9C-B0D9-C9C2648545D9}"/>
-    <hyperlink ref="F14" r:id="rId5" xr:uid="{DD4FF0E3-EAE0-469C-ACDD-C865EBB378ED}"/>
-    <hyperlink ref="G14" r:id="rId6" xr:uid="{7C8E9920-0270-4770-84B0-00A2DD3F4658}"/>
-    <hyperlink ref="I14" r:id="rId7" xr:uid="{7002ECE4-5F74-45CB-8AAA-D54AAD68F48C}"/>
-    <hyperlink ref="J14" r:id="rId8" xr:uid="{A952527B-8DAC-4C2B-BB35-4E0F883A762B}"/>
-    <hyperlink ref="K14" r:id="rId9" xr:uid="{03970A6A-02B7-44F7-86E2-F33B08E4D592}"/>
-    <hyperlink ref="H14" r:id="rId10" xr:uid="{28BD77ED-2D3E-4929-BB52-7E05B9F6BC04}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{3945B433-F36A-47F7-81F3-3217A70B44EA}"/>
+    <hyperlink ref="D13" r:id="rId3" xr:uid="{66EC8D73-7E0C-46A6-B289-AC037C945EBA}"/>
+    <hyperlink ref="E13" r:id="rId4" xr:uid="{37E5CC3F-B59C-4D9C-B0D9-C9C2648545D9}"/>
+    <hyperlink ref="F13" r:id="rId5" xr:uid="{DD4FF0E3-EAE0-469C-ACDD-C865EBB378ED}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{7C8E9920-0270-4770-84B0-00A2DD3F4658}"/>
+    <hyperlink ref="H13" r:id="rId7" xr:uid="{7002ECE4-5F74-45CB-8AAA-D54AAD68F48C}"/>
+    <hyperlink ref="I13" r:id="rId8" xr:uid="{A952527B-8DAC-4C2B-BB35-4E0F883A762B}"/>
+    <hyperlink ref="J13" r:id="rId9" xr:uid="{03970A6A-02B7-44F7-86E2-F33B08E4D592}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
-  <drawing r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -2908,417 +2826,417 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976A494-BCBD-49B6-B4BB-BF67D4A68194}">
   <dimension ref="A2:M21"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" style="41" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="44.7265625" style="39" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" style="39" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" style="39" customWidth="1"/>
-    <col min="6" max="6" width="23.54296875" style="39" customWidth="1"/>
-    <col min="7" max="7" width="32.08984375" style="39" customWidth="1"/>
-    <col min="8" max="8" width="20.26953125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" style="39" customWidth="1"/>
-    <col min="10" max="10" width="60.08984375" style="48" customWidth="1"/>
-    <col min="11" max="11" width="56.54296875" style="67" customWidth="1"/>
-    <col min="12" max="13" width="8.7265625" style="48"/>
-    <col min="14" max="16384" width="8.7265625" style="39"/>
+    <col min="1" max="1" width="20.53125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="38.796875" style="40" customWidth="1"/>
+    <col min="3" max="3" width="44.73046875" style="40" customWidth="1"/>
+    <col min="4" max="4" width="30.59765625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="44.796875" style="40" customWidth="1"/>
+    <col min="6" max="6" width="23.53125" style="40" customWidth="1"/>
+    <col min="7" max="7" width="32.06640625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="20.265625" style="40" customWidth="1"/>
+    <col min="9" max="9" width="21.53125" style="40" customWidth="1"/>
+    <col min="10" max="10" width="60.06640625" style="49" customWidth="1"/>
+    <col min="11" max="11" width="56.53125" style="68" customWidth="1"/>
+    <col min="12" max="13" width="8.73046875" style="49"/>
+    <col min="14" max="16384" width="8.73046875" style="40"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:13" s="40" customFormat="1" ht="142" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="82" t="s">
+    <row r="2" spans="1:13" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65"/>
+    <row r="3" spans="1:13" s="41" customFormat="1" ht="142.05000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="68" t="s">
+      <c r="K3" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-    </row>
-    <row r="4" spans="1:13" ht="233" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="83" t="s">
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+    </row>
+    <row r="4" spans="1:13" ht="233" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A4" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="75" t="s">
+      <c r="F4" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="78"/>
-    </row>
-    <row r="5" spans="1:13" ht="159.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="84" t="s">
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:13" ht="159.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="70" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="71" t="s">
+      <c r="C5" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="71" t="s">
+      <c r="F5" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="72" t="s">
+      <c r="H5" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="K5" s="75" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="134" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="65" t="s">
+    <row r="6" spans="1:13" ht="134" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="46" t="s">
+      <c r="B6" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="43" t="s">
+      <c r="D6" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="55" t="s">
+      <c r="K6" s="56" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="49.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="65" t="s">
+    <row r="7" spans="1:13" ht="49.5" x14ac:dyDescent="0.6">
+      <c r="A7" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="1:13" ht="193" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="65" t="s">
+      <c r="K7" s="56"/>
+    </row>
+    <row r="8" spans="1:13" ht="193.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="44" t="s">
+      <c r="B8" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="42" t="s">
+      <c r="E8" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="K8" s="54" t="s">
+      <c r="K8" s="55" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="199" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="65" t="s">
+    <row r="9" spans="1:13" ht="199.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="46" t="s">
+      <c r="D9" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="43" t="s">
+      <c r="F9" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="49" t="s">
+      <c r="J9" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="69" t="s">
+      <c r="K9" s="70" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="180" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="65" t="s">
+    <row r="10" spans="1:13" ht="180" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="44" t="s">
+      <c r="E10" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="54" t="s">
+      <c r="K10" s="55" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="63.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="65" t="s">
+    <row r="11" spans="1:13" ht="63.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="K11" s="55" t="s">
+      <c r="K11" s="56" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="216.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="66" t="s">
+    <row r="12" spans="1:13" ht="216.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A12" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="57" t="s">
+      <c r="D12" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="K12" s="61" t="s">
+      <c r="K12" s="62" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.6">
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.6">
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.6">
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.6">
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.6">
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.6">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.6">
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.6">
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.6">
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3337,23 +3255,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="9f9f0ed7-b6e7-4e0d-9b4d-b4e73fb1e1ba" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F4EB56A014601647A8A96FC1FEAD7A4D" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ce20bcdb31e35f84e91aaebcc88b9c29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9f9f0ed7-b6e7-4e0d-9b4d-b4e73fb1e1ba" xmlns:ns3="5d0a0686-a3c6-401e-8596-31c6446e2673" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a5f8733a3652043e24787deaf46a0bd" ns2:_="" ns3:_="">
     <xsd:import namespace="9f9f0ed7-b6e7-4e0d-9b4d-b4e73fb1e1ba"/>
@@ -3538,10 +3439,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="9f9f0ed7-b6e7-4e0d-9b4d-b4e73fb1e1ba" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{317DBB47-F340-434F-9FE6-0BC3D8459AF6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7742B622-1320-460F-82D3-3D60BC8B68F7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9f9f0ed7-b6e7-4e0d-9b4d-b4e73fb1e1ba"/>
+    <ds:schemaRef ds:uri="5d0a0686-a3c6-401e-8596-31c6446e2673"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3564,20 +3493,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7742B622-1320-460F-82D3-3D60BC8B68F7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{317DBB47-F340-434F-9FE6-0BC3D8459AF6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9f9f0ed7-b6e7-4e0d-9b4d-b4e73fb1e1ba"/>
-    <ds:schemaRef ds:uri="5d0a0686-a3c6-401e-8596-31c6446e2673"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>